<commit_message>
done backedn testing time
</commit_message>
<xml_diff>
--- a/src/python/IDP_DATA_MENTEE.xlsx
+++ b/src/python/IDP_DATA_MENTEE.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="14400" windowHeight="12900" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="28800" windowHeight="12885" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mentee" sheetId="1" state="visible" r:id="rId1"/>
@@ -1434,7 +1434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2119,7 +2119,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>axl</t>
+          <t>Trường hợp 1</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>Kinh doanh quốc tế</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2141,17 +2141,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>hhs</t>
+          <t>Trường hợp 2</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Hóa mỹ phẩm</t>
+          <t>Tín dụng ngân hàng</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2163,7 +2163,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>hhs</t>
+          <t>Trường hợp 3</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2173,10 +2173,120 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Hóa vô cơ</t>
+          <t>Web development</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Trường hợp 3</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Web development</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Trường hợp 3</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>An toàn ứng dụng</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Trường hợp 4</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Ngân hàng thương mại</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Trường hợp 5</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Content creator</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Trường hợp 5</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Nữ</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Content creator</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
         <is>
           <t>Mentee</t>
         </is>

</xml_diff>

<commit_message>
Add src/python/model to .gitignore
</commit_message>
<xml_diff>
--- a/src/python/IDP_DATA_MENTEE.xlsx
+++ b/src/python/IDP_DATA_MENTEE.xlsx
@@ -1434,7 +1434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2287,6 +2287,270 @@
         </is>
       </c>
       <c r="D39" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>acsg</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Nữ</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>An ninh mạng</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>acsg</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Công nghệ thông tin</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>BÙI XUÂN LỘC</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Công nghệ thông tin</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>BÙI XUÂN LỘC</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>BÙI XUÂN LỘC</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Nữ</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>abc1</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Nữ</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>abc2</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Nữ</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>abc3</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Nữ</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>abc4</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Nữ</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Mentee</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ABCS</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>An ninh mạng</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
         <is>
           <t>Mentee</t>
         </is>

</xml_diff>

<commit_message>
Bo sung admin frame
</commit_message>
<xml_diff>
--- a/src/python/IDP_DATA_MENTEE.xlsx
+++ b/src/python/IDP_DATA_MENTEE.xlsx
@@ -1649,15 +1649,10 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="A31" sqref="$A31:$XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="9.57142857142857" customWidth="1"/>
-    <col min="3" max="3" width="37.5714285714286" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="40" t="s">

</xml_diff>